<commit_message>
Add geometry in ahtlete_0
</commit_message>
<xml_diff>
--- a/doc/Planning.xlsx
+++ b/doc/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcelhacker/Documents/opensim-deadlift-techniques/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D538B20-E543-BE4E-A68B-676CA884F9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B793314C-6DC1-9D46-AADB-8CACF7BEB292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16680" xr2:uid="{D596EE47-F267-354E-8852-8744F315EF1A}"/>
   </bookViews>
@@ -828,7 +828,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>

</xml_diff>